<commit_message>
- Új hetek dokumentálása
</commit_message>
<xml_diff>
--- a/Dokumentációk/Megbeszélések és Esemény napló/Chat dokumentálás.xlsx
+++ b/Dokumentációk/Megbeszélések és Esemény napló/Chat dokumentálás.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Archived\MilliomosProject\Miliomos_Project\Dokumentációk\Megbeszélések és Esemény napló\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Archived\MilliomosProject\Miliomos_Project\Dokumentációk\Megbeszélések és Esemény napló\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA966A0-377E-427B-8C2C-FE7327C41671}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEB67074-C94C-4624-9309-E1670BDD417F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-1380" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="62">
   <si>
     <t>Dátum</t>
   </si>
@@ -100,103 +100,10 @@
     <t>10. hét</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t>Keddi személyes összejövetel</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t>: Csoport összejövetelek időpontjai, ki miben tudna részt venni (back-end, front-end), Facebook csoportba való meghívás, Jövőhétre való készületek.</t>
-    </r>
-  </si>
-  <si>
     <t>https://dl.dropboxusercontent.com/s/r0x52ape6ghnt8h/chrome_ZJDwQiUWSu.png</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t>Online:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> Project megszervezése, Ideiglenes Facebook csoport megbeszélésekre, Online "raktár" repository létrehozása(GIT) / Elvállalt feladatok megszervezése/ Management - Nagy Ádám // Front és back-end felkészülések, hivatkozások alapján tanulás - Bajnok Tamás + Tóth Tamás + Varsa Laci // Chat és megbeszélések dokumentálása, ideiglenesen google docs segítségével - Szabó Attila // Regisztráció + Login alap elkezdése - Bajnok Tamás // Design teszt gráf (melléklet 1.) - Varsa Laci</t>
-    </r>
-  </si>
-  <si>
     <t>https://dl.dropboxusercontent.com/s/08gsh8gyt3vk8a0/chrome_I44cO1ndDG.png</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t>Szombati összejövetel</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t>: 11:00-kor Online: Első megbeszélés. Csapat név eldöntése. Adatbázis terv excel létrehozása (git-re feltöltése) - Tóth Tamás, Chat dokumentálása/Git használat dokumentálásának elkezdése - Szabó Attila, Git-elérés biztosítása és alapok feltöltése - Nagy Ádám</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t>Egyéb megjegyzések</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t xml:space="preserve">: Következő személyes megbeszélésen back-end és front-end alapjainak megbeszélése. Probléma elkerülése érdekében a program felépítésének áttekintése (verzió kezelés). </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t>Határidőn belül elküldeni a tanárnőnek a beadandó dokumentumot (nevek/választott project)</t>
-    </r>
   </si>
   <si>
     <r>
@@ -705,6 +612,262 @@
         <charset val="238"/>
       </rPr>
       <t>Scoreboard legyen meg jövőhétre!</t>
+    </r>
+  </si>
+  <si>
+    <t>Egyéb megjegyzések: Highscore frontend legyen kész</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>Online összejövetel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>: Funkciók bővítése</t>
+    </r>
+  </si>
+  <si>
+    <t>Egyéb megjegyzések: Dokumentálás 30 oldal+ legyen meg</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>Online összejövetel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>: ScoreBord görgethetősége
+Offline verzió 
+kinézet átdolgozása
+kérdések bővítése(kérdés db) 
+25 kérdéses verzió
+Due Verzio</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Egyéb megjegyzések: </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>Online:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>Online:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> Védelem, Offline verzió</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">, PROJECT JELENLÉTI </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Egyéb megjegyzések: Highscore frontend legyen kész, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>PROJECT JELENTÉS FELTÖLTÉSE</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>Online összejövetel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>: Funkciók bővítése, Front End bővítése</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>Keddi személyes összejövetel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>: ZH után megbeszélés röviden, Dokumentálásal kapcsolatos tudnivalók, formai dolgok, Dokumentálás részeinek kiosztása.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>Online:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve"> Project megszervezése, Ideiglenes Facebook csoport megbeszélésekre, Online "raktár" repository létrehozása(GIT) / Elvállalt feladatok megszervezése/ Management - Nagy Ádám // Front és back-end felkészülések, hivatkozások alapján tanulás - Bajnok Tamás + Tóth Tamás + Varsa Laci // Chat és megbeszélések dokumentálása, ideiglenesen google docs segítségével - Szabó Attila // Regisztráció + Login alap elkezdése - Bajnok Tamás // Design teszt gráf (melléklet 1.) - Varsa Laci</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>Keddi személyes összejövetel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>: Csoport összejövetelek időpontjai, ki miben tudna részt venni (back-end, front-end), Facebook csoportba való meghívás, Jövőhétre való készületek.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>Szombati összejövetel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>: 11:00-kor Online: Első megbeszélés. Csapat név eldöntése. Adatbázis terv excel létrehozása (git-re feltöltése) - Tóth Tamás, Chat dokumentálása/Git használat dokumentálásának elkezdése - Szabó Attila, Git-elérés biztosítása és alapok feltöltése - Nagy Ádám</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>Egyéb megjegyzések</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">: Következő személyes megbeszélésen back-end és front-end alapjainak megbeszélése. Probléma elkerülése érdekében a program felépítésének áttekintése (verzió kezelés). </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>Határidőn belül elküldeni a tanárnőnek a beadandó dokumentumot (nevek/választott project)</t>
     </r>
   </si>
 </sst>
@@ -712,7 +875,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -775,6 +938,35 @@
       <b/>
       <sz val="11"/>
       <color theme="9" tint="-0.249977111117893"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="238"/>
@@ -936,17 +1128,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -959,18 +1142,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -989,12 +1160,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1007,14 +1172,71 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1334,11 +1556,9 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B1:E27"/>
+  <dimension ref="B1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1351,277 +1571,389 @@
   <sheetData>
     <row r="1" spans="2:5" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="2:5" ht="114.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="11"/>
+      <c r="E3" s="23"/>
     </row>
     <row r="4" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="28"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="28"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="32"/>
+    </row>
+    <row r="7" spans="2:5" ht="114.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="33"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="36"/>
+    </row>
+    <row r="8" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="12"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="21"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="21"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="4"/>
-    </row>
-    <row r="7" spans="2:5" ht="114.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="22"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="5" t="s">
+      <c r="E9" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="12"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="18"/>
-    </row>
-    <row r="8" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="16" t="s">
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="2:5" ht="114.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="13"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="21"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="7" t="s">
+      <c r="E12" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="12"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E13" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="12"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" ht="114.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="13"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="9" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="10" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="21"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="2:5" ht="114.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="22"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="6"/>
-    </row>
-    <row r="12" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="E12" s="17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="21"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" s="4" t="s">
+      <c r="E16" s="10"/>
+    </row>
+    <row r="17" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="12"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="4" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="14" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="21"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E14" s="4" t="s">
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="12"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="2:5" ht="114.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="13"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="10"/>
+    </row>
+    <row r="21" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="12"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="12"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="2:5" ht="114.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="13"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="15" spans="2:5" ht="114.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="22"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" s="6"/>
-    </row>
-    <row r="16" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="E16" s="17"/>
-    </row>
-    <row r="17" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="21"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="7" t="s">
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="21"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="7" t="s">
+      <c r="E24" s="10"/>
+    </row>
+    <row r="25" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="12"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="2:5" ht="114.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="22"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="5" t="s">
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="12"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="2:5" ht="114.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="13"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E28" s="10"/>
+    </row>
+    <row r="29" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="12"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="12"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="2:5" ht="114.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="13"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E32" s="10"/>
+    </row>
+    <row r="33" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="12"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="12"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E19" s="6"/>
-    </row>
-    <row r="20" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="D20" s="16" t="s">
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="2:5" ht="114.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="13"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="E35" s="3"/>
+    </row>
+    <row r="36" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E36" s="10"/>
+    </row>
+    <row r="37" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="12"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E37" s="1"/>
+    </row>
+    <row r="38" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="12"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="2:5" ht="114.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="13"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="E20" s="17"/>
-    </row>
-    <row r="21" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="21"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="E21" s="4"/>
-    </row>
-    <row r="22" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="21"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E22" s="4"/>
-    </row>
-    <row r="23" spans="2:5" ht="114.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="22"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E23" s="6"/>
-    </row>
-    <row r="24" spans="2:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D24" s="2"/>
-      <c r="E24" s="3"/>
-    </row>
-    <row r="25" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D25" s="2"/>
-      <c r="E25" s="3"/>
-    </row>
-    <row r="26" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D26" s="2"/>
-      <c r="E26" s="3"/>
-    </row>
-    <row r="27" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D27" s="2"/>
-      <c r="E27" s="3"/>
+      <c r="E39" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="18">
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="C32:C35"/>
     <mergeCell ref="B16:B19"/>
     <mergeCell ref="C16:C19"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="C36:C39"/>
     <mergeCell ref="B4:B7"/>
     <mergeCell ref="C4:C7"/>
     <mergeCell ref="B12:B15"/>
     <mergeCell ref="C12:C15"/>
     <mergeCell ref="B8:B11"/>
     <mergeCell ref="C8:C11"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="C28:C31"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E4" r:id="rId1" xr:uid="{0C6D9F65-035A-46DB-BD55-C1313CA33086}"/>

</xml_diff>